<commit_message>
Added standard division ('region' label = [1,5])
</commit_message>
<xml_diff>
--- a/data/output_example/mesh_clip_planes.xlsx
+++ b/data/output_example/mesh_clip_planes.xlsx
@@ -348,13 +348,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1">
-        <v>176.5290069580078</v>
+        <v>175.8354644775391</v>
       </c>
       <c r="B1">
-        <v>202.5780944824219</v>
+        <v>204.3758087158203</v>
       </c>
       <c r="C1">
-        <v>53.45513534545898</v>
+        <v>53.14113235473633</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -370,13 +370,13 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>175.6315460205078</v>
+        <v>173.7902374267578</v>
       </c>
       <c r="B3">
-        <v>191.3430938720703</v>
+        <v>191.04052734375</v>
       </c>
       <c r="C3">
-        <v>73.14945220947266</v>
+        <v>73.91013336181641</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -392,13 +392,13 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>233.5271759033203</v>
+        <v>235.4834136962891</v>
       </c>
       <c r="B5">
-        <v>200.3733673095703</v>
+        <v>200.2127685546875</v>
       </c>
       <c r="C5">
-        <v>82.77371978759766</v>
+        <v>83.19190216064453</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -414,13 +414,13 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>232.9117126464844</v>
+        <v>234.7833709716797</v>
       </c>
       <c r="B7">
-        <v>210.6747131347656</v>
+        <v>211.2177734375</v>
       </c>
       <c r="C7">
-        <v>66.51792907714844</v>
+        <v>66.07094573974609</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -436,13 +436,13 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>237.9435729980469</v>
+        <v>238.6244354248047</v>
       </c>
       <c r="B9">
-        <v>183.0521392822266</v>
+        <v>182.9368133544922</v>
       </c>
       <c r="C9">
-        <v>76.12953186035156</v>
+        <v>77.99478912353516</v>
       </c>
     </row>
     <row r="10" spans="1:3">

</xml_diff>